<commit_message>
Added new Testcase AddBooks to user
</commit_message>
<xml_diff>
--- a/src/test/resources/Suites/Suites.xlsx
+++ b/src/test/resources/Suites/Suites.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Test Case #</t>
   </si>
@@ -99,6 +99,19 @@
   </si>
   <si>
     <t>/BookStore/v1/Books</t>
+  </si>
+  <si>
+    <t>AddBooks</t>
+  </si>
+  <si>
+    <t>{
+  "userId": "string",
+  "collectionOfIsbns": [
+    {
+      "isbn": "9781449325862"
+    }
+  ]
+}</t>
   </si>
 </sst>
 </file>
@@ -454,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,6 +585,23 @@
         <v>23</v>
       </c>
     </row>
+    <row r="7" spans="1:13" ht="174" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>